<commit_message>
Organizando la parte de la deformada y su escala
</commit_message>
<xml_diff>
--- a/codigo/losas/ejemplos/losa_rectangular_libro_solidos_efQ4.xlsx
+++ b/codigo/losas/ejemplos/losa_rectangular_libro_solidos_efQ4.xlsx
@@ -435,7 +435,7 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="6.23"/>
@@ -9972,7 +9972,7 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="11.52"/>
@@ -23839,7 +23839,7 @@
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.66"/>
   </cols>
@@ -28364,10 +28364,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -28468,7 +28468,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>